<commit_message>
Update attached file to reflect the most current information available
Replace existing file with a newer version to ensure data accuracy.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: fb3f09bb-ebf3-4e03-b013-b640d7f63b45
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ebf6d994-e003-4241-a204-74c5ddc9bda0/915663c7-75cf-4a62-a1c6-a611e7592f50.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Test Tracker 2024-2025.xlsx
+++ b/attached_assets/Test Tracker 2024-2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Munye\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Munye\Desktop\NFS English Language School\GOVCIO Test Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B2FBD29-2682-4C27-A99B-BEE3CCACF90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0CFEB2-6659-42E1-A47B-35432B15A6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="782" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALCPT SCORES" sheetId="6" r:id="rId1"/>
@@ -1554,10 +1554,6 @@
     <xf numFmtId="0" fontId="14" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1617,6 +1613,10 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4600,7 +4600,7 @@
   </sheetPr>
   <dimension ref="A1:IO144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
@@ -4630,36 +4630,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="102"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="101"/>
     </row>
     <row r="2" spans="1:39" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
@@ -4748,36 +4748,36 @@
       </c>
     </row>
     <row r="3" spans="1:39" s="25" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="105"/>
-      <c r="Z3" s="105"/>
-      <c r="AA3" s="105"/>
-      <c r="AB3" s="105"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+      <c r="AB3" s="104"/>
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -7032,36 +7032,36 @@
       <c r="AB30" s="2"/>
     </row>
     <row r="31" spans="1:249" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="103"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-      <c r="T31" s="103"/>
-      <c r="U31" s="103"/>
-      <c r="V31" s="103"/>
-      <c r="W31" s="103"/>
-      <c r="X31" s="103"/>
-      <c r="Y31" s="103"/>
-      <c r="Z31" s="103"/>
-      <c r="AA31" s="103"/>
-      <c r="AB31" s="103"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+      <c r="N31" s="102"/>
+      <c r="O31" s="102"/>
+      <c r="P31" s="102"/>
+      <c r="Q31" s="102"/>
+      <c r="R31" s="102"/>
+      <c r="S31" s="102"/>
+      <c r="T31" s="102"/>
+      <c r="U31" s="102"/>
+      <c r="V31" s="102"/>
+      <c r="W31" s="102"/>
+      <c r="X31" s="102"/>
+      <c r="Y31" s="102"/>
+      <c r="Z31" s="102"/>
+      <c r="AA31" s="102"/>
+      <c r="AB31" s="102"/>
     </row>
     <row r="32" spans="1:249" s="88" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="74">
@@ -7964,36 +7964,36 @@
       <c r="IO34"/>
     </row>
     <row r="35" spans="1:249" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="104" t="s">
+      <c r="A35" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="104"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="104"/>
-      <c r="E35" s="104"/>
-      <c r="F35" s="104"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="104"/>
-      <c r="L35" s="104"/>
-      <c r="M35" s="104"/>
-      <c r="N35" s="104"/>
-      <c r="O35" s="104"/>
-      <c r="P35" s="104"/>
-      <c r="Q35" s="104"/>
-      <c r="R35" s="104"/>
-      <c r="S35" s="104"/>
-      <c r="T35" s="104"/>
-      <c r="U35" s="104"/>
-      <c r="V35" s="104"/>
-      <c r="W35" s="104"/>
-      <c r="X35" s="104"/>
-      <c r="Y35" s="104"/>
-      <c r="Z35" s="104"/>
-      <c r="AA35" s="104"/>
-      <c r="AB35" s="104"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="103"/>
+      <c r="K35" s="103"/>
+      <c r="L35" s="103"/>
+      <c r="M35" s="103"/>
+      <c r="N35" s="103"/>
+      <c r="O35" s="103"/>
+      <c r="P35" s="103"/>
+      <c r="Q35" s="103"/>
+      <c r="R35" s="103"/>
+      <c r="S35" s="103"/>
+      <c r="T35" s="103"/>
+      <c r="U35" s="103"/>
+      <c r="V35" s="103"/>
+      <c r="W35" s="103"/>
+      <c r="X35" s="103"/>
+      <c r="Y35" s="103"/>
+      <c r="Z35" s="103"/>
+      <c r="AA35" s="103"/>
+      <c r="AB35" s="103"/>
     </row>
     <row r="36" spans="1:249" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
@@ -8940,36 +8940,36 @@
       <c r="AB51" s="2"/>
     </row>
     <row r="52" spans="1:223" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="104" t="s">
+      <c r="A52" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="104"/>
-      <c r="C52" s="104"/>
-      <c r="D52" s="104"/>
-      <c r="E52" s="104"/>
-      <c r="F52" s="104"/>
-      <c r="G52" s="104"/>
-      <c r="H52" s="104"/>
-      <c r="I52" s="104"/>
-      <c r="J52" s="104"/>
-      <c r="K52" s="104"/>
-      <c r="L52" s="104"/>
-      <c r="M52" s="104"/>
-      <c r="N52" s="104"/>
-      <c r="O52" s="104"/>
-      <c r="P52" s="104"/>
-      <c r="Q52" s="104"/>
-      <c r="R52" s="104"/>
-      <c r="S52" s="104"/>
-      <c r="T52" s="104"/>
-      <c r="U52" s="104"/>
-      <c r="V52" s="104"/>
-      <c r="W52" s="104"/>
-      <c r="X52" s="104"/>
-      <c r="Y52" s="104"/>
-      <c r="Z52" s="104"/>
-      <c r="AA52" s="104"/>
-      <c r="AB52" s="104"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="103"/>
+      <c r="J52" s="103"/>
+      <c r="K52" s="103"/>
+      <c r="L52" s="103"/>
+      <c r="M52" s="103"/>
+      <c r="N52" s="103"/>
+      <c r="O52" s="103"/>
+      <c r="P52" s="103"/>
+      <c r="Q52" s="103"/>
+      <c r="R52" s="103"/>
+      <c r="S52" s="103"/>
+      <c r="T52" s="103"/>
+      <c r="U52" s="103"/>
+      <c r="V52" s="103"/>
+      <c r="W52" s="103"/>
+      <c r="X52" s="103"/>
+      <c r="Y52" s="103"/>
+      <c r="Z52" s="103"/>
+      <c r="AA52" s="103"/>
+      <c r="AB52" s="103"/>
     </row>
     <row r="53" spans="1:223" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7">
@@ -13062,31 +13062,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="102"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="101"/>
     </row>
     <row r="2" spans="1:23" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -13160,31 +13160,31 @@
       </c>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="107"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="106"/>
     </row>
     <row r="4" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
@@ -14996,31 +14996,31 @@
       <c r="W30" s="7"/>
     </row>
     <row r="31" spans="1:23" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="106" t="s">
+      <c r="A31" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="105"/>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="105"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="105"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="105"/>
-      <c r="M31" s="105"/>
-      <c r="N31" s="105"/>
-      <c r="O31" s="105"/>
-      <c r="P31" s="105"/>
-      <c r="Q31" s="105"/>
-      <c r="R31" s="105"/>
-      <c r="S31" s="105"/>
-      <c r="T31" s="105"/>
-      <c r="U31" s="105"/>
-      <c r="V31" s="105"/>
-      <c r="W31" s="107"/>
+      <c r="B31" s="104"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="104"/>
+      <c r="N31" s="104"/>
+      <c r="O31" s="104"/>
+      <c r="P31" s="104"/>
+      <c r="Q31" s="104"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="104"/>
+      <c r="T31" s="104"/>
+      <c r="U31" s="104"/>
+      <c r="V31" s="104"/>
+      <c r="W31" s="106"/>
     </row>
     <row r="32" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
@@ -15212,31 +15212,31 @@
       <c r="W34" s="7"/>
     </row>
     <row r="35" spans="1:23" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="105"/>
-      <c r="N35" s="105"/>
-      <c r="O35" s="105"/>
-      <c r="P35" s="105"/>
-      <c r="Q35" s="105"/>
-      <c r="R35" s="105"/>
-      <c r="S35" s="105"/>
-      <c r="T35" s="105"/>
-      <c r="U35" s="105"/>
-      <c r="V35" s="105"/>
-      <c r="W35" s="107"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="104"/>
+      <c r="L35" s="104"/>
+      <c r="M35" s="104"/>
+      <c r="N35" s="104"/>
+      <c r="O35" s="104"/>
+      <c r="P35" s="104"/>
+      <c r="Q35" s="104"/>
+      <c r="R35" s="104"/>
+      <c r="S35" s="104"/>
+      <c r="T35" s="104"/>
+      <c r="U35" s="104"/>
+      <c r="V35" s="104"/>
+      <c r="W35" s="106"/>
     </row>
     <row r="36" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
@@ -16121,31 +16121,31 @@
       <c r="W53" s="7"/>
     </row>
     <row r="54" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="108" t="s">
+      <c r="A54" s="107" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="109"/>
-      <c r="C54" s="109"/>
-      <c r="D54" s="109"/>
-      <c r="E54" s="109"/>
-      <c r="F54" s="109"/>
-      <c r="G54" s="109"/>
-      <c r="H54" s="109"/>
-      <c r="I54" s="109"/>
-      <c r="J54" s="109"/>
-      <c r="K54" s="109"/>
-      <c r="L54" s="109"/>
-      <c r="M54" s="109"/>
-      <c r="N54" s="109"/>
-      <c r="O54" s="109"/>
-      <c r="P54" s="109"/>
-      <c r="Q54" s="109"/>
-      <c r="R54" s="109"/>
-      <c r="S54" s="109"/>
-      <c r="T54" s="109"/>
-      <c r="U54" s="109"/>
-      <c r="V54" s="109"/>
-      <c r="W54" s="110"/>
+      <c r="B54" s="108"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="108"/>
+      <c r="K54" s="108"/>
+      <c r="L54" s="108"/>
+      <c r="M54" s="108"/>
+      <c r="N54" s="108"/>
+      <c r="O54" s="108"/>
+      <c r="P54" s="108"/>
+      <c r="Q54" s="108"/>
+      <c r="R54" s="108"/>
+      <c r="S54" s="108"/>
+      <c r="T54" s="108"/>
+      <c r="U54" s="108"/>
+      <c r="V54" s="108"/>
+      <c r="W54" s="109"/>
     </row>
     <row r="55" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="45">
@@ -16575,31 +16575,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="114"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="113"/>
     </row>
     <row r="2" spans="1:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -16673,31 +16673,31 @@
       </c>
     </row>
     <row r="3" spans="1:26" s="26" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="112"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="111"/>
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
@@ -17736,31 +17736,31 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="111" t="s">
+      <c r="A31" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="103"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-      <c r="T31" s="103"/>
-      <c r="U31" s="103"/>
-      <c r="V31" s="103"/>
-      <c r="W31" s="112"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="102"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="102"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="102"/>
+      <c r="M31" s="102"/>
+      <c r="N31" s="102"/>
+      <c r="O31" s="102"/>
+      <c r="P31" s="102"/>
+      <c r="Q31" s="102"/>
+      <c r="R31" s="102"/>
+      <c r="S31" s="102"/>
+      <c r="T31" s="102"/>
+      <c r="U31" s="102"/>
+      <c r="V31" s="102"/>
+      <c r="W31" s="111"/>
     </row>
     <row r="32" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
@@ -20895,7 +20895,7 @@
   </sheetPr>
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -20922,31 +20922,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="59.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="116"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="115"/>
     </row>
     <row r="2" spans="1:27" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
@@ -21020,31 +21020,31 @@
       </c>
     </row>
     <row r="3" spans="1:27" s="27" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="107"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="106"/>
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
@@ -21519,7 +21519,7 @@
       <c r="C17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="119" t="s">
         <v>111</v>
       </c>
       <c r="E17" s="43" t="s">
@@ -21554,7 +21554,7 @@
       <c r="C18" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="99" t="s">
+      <c r="D18" s="119" t="s">
         <v>111</v>
       </c>
       <c r="E18" s="43" t="s">
@@ -22190,28 +22190,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="119" t="s">
+      <c r="E1" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="116" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="10" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="117"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="116"/>
     </row>
     <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="61">
@@ -22454,11 +22454,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="116"/>
       <c r="D19" s="63" t="s">
         <v>90</v>
       </c>
@@ -22598,11 +22598,11 @@
       <c r="F27" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="117" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
       <c r="D29" s="63" t="s">
         <v>82</v>
       </c>

</xml_diff>